<commit_message>
Avatar p1, merge conflicts
</commit_message>
<xml_diff>
--- a/Feature list.xlsx
+++ b/Feature list.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10116"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\User\Desktop\Year 4\Final Project\Social-Vr\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/Apple SSD AP0032H/Social-Vr/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C227AE2-9E32-4BDB-AB55-CFE3F3E87CBB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5739CD31-78C5-5F4C-9232-C6FC74940585}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{B090C440-03CE-4D42-84C1-91E7B2F52996}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="29040" windowHeight="15720" xr2:uid="{B090C440-03CE-4D42-84C1-91E7B2F52996}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -140,7 +140,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -177,6 +177,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF8FCC4F"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -190,7 +196,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -198,11 +204,108 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="4">
+  <dxfs count="16">
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF92D050"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF9BC2E6"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFE699"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFF4B084"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF92D050"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF9BC2E6"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFE699"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFF4B084"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF92D050"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF9BC2E6"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFE699"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFF4B084"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill patternType="solid">
@@ -237,6 +340,12 @@
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FF8FCC4F"/>
+      <color rgb="FF92D051"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -547,19 +656,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F18F3099-0489-4625-BBD3-EAAD0CB89B75}">
   <dimension ref="A2:F20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+    <sheetView tabSelected="1" zoomScale="156" workbookViewId="0">
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="18.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="47.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="47.5" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="29" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:6" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:6" ht="24" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>10</v>
       </c>
@@ -573,117 +682,117 @@
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B3" s="2" t="s">
-        <v>0</v>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B3" s="6" t="s">
+        <v>17</v>
       </c>
       <c r="F3" s="2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B4" s="2" t="s">
-        <v>19</v>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B4" s="6" t="s">
+        <v>2</v>
       </c>
       <c r="F4" s="3" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B5" s="6" t="s">
-        <v>24</v>
+        <v>3</v>
       </c>
       <c r="F5" s="4" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B6" s="6" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B7" s="6" t="s">
-        <v>2</v>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B7" s="4" t="s">
+        <v>9</v>
       </c>
       <c r="F7" s="5" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B8" s="6" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B9" s="6" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B10" s="6" t="s">
-        <v>5</v>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B8" s="4" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B9" s="4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B10" s="7" t="s">
+        <v>0</v>
       </c>
       <c r="C10" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B11" s="6" t="s">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B11" s="7" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B12" s="7" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B13" s="7" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B14" s="7" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B12" s="4" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B13" s="4" t="s">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B15" s="7" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B14" s="4" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B15" s="4" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B16" s="4" t="s">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B16" s="7" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="17" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B17" s="5" t="s">
+    <row r="17" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B17" s="7" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="18" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B18" s="7" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="19" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B19" s="5" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="18" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B18" s="5" t="s">
+    <row r="20" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B20" s="5" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="19" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B19" s="2" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="20" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B20" s="2" t="s">
-        <v>26</v>
-      </c>
-    </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B2:B18">
-    <sortCondition sortBy="cellColor" ref="B2:B18" dxfId="3"/>
-    <sortCondition sortBy="cellColor" ref="B2:B18" dxfId="2"/>
-    <sortCondition sortBy="cellColor" ref="B2:B18" dxfId="1"/>
-    <sortCondition descending="1" sortBy="cellColor" ref="B2:B18" dxfId="0"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B3:B20">
+    <sortCondition sortBy="cellColor" ref="B3:B20" dxfId="7"/>
+    <sortCondition sortBy="cellColor" ref="B3:B20" dxfId="6"/>
+    <sortCondition sortBy="cellColor" ref="B3:B20" dxfId="5"/>
+    <sortCondition descending="1" sortBy="cellColor" ref="B3:B20" dxfId="4"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>

</xml_diff>